<commit_message>
Updated R1 on schematic, Updated R1 on BOM, add alt for button
</commit_message>
<xml_diff>
--- a/hardware/datasheets/BOM_Rev1.xlsx
+++ b/hardware/datasheets/BOM_Rev1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/033a6759af201263/School/SS 2021/EE 491/Git Repository/sddec21-07/hardware/datasheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parker\Desktop\SeniorDesign\sddec21-07\hardware\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="305" documentId="8_{E1C920AF-5021-4130-838C-A443A4E78260}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4BB78C11-0828-446F-9E49-B11F8330990B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98980E69-2DCF-4B67-8E4A-2A02206E9BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21840" yWindow="-16530" windowWidth="19215" windowHeight="12945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zigbeeCape" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="248">
   <si>
     <t>Reference</t>
   </si>
@@ -211,12 +211,6 @@
     <t>10nH</t>
   </si>
   <si>
-    <t xml:space="preserve">R1 </t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
     <t xml:space="preserve">R17 R19 </t>
   </si>
   <si>
@@ -229,9 +223,6 @@
     <t>10K</t>
   </si>
   <si>
-    <t xml:space="preserve">R3 </t>
-  </si>
-  <si>
     <t>DNM_10K</t>
   </si>
   <si>
@@ -764,6 +755,15 @@
   </si>
   <si>
     <t>https://suntsu.com/wp-content/uploads/2020/07/SXT324-Series-1.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1 R3 </t>
+  </si>
+  <si>
+    <t>Parts not mounted</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/e-switch/TL3305CF160QG/5816183</t>
   </si>
 </sst>
 </file>
@@ -1662,21 +1662,21 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" customWidth="1"/>
-    <col min="6" max="6" width="56.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="56.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="77.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="77.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1693,19 +1693,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1716,10 +1716,10 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1730,25 +1730,25 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1759,25 +1759,25 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1788,25 +1788,25 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="H5" t="s">
-        <v>120</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1817,25 +1817,25 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1846,25 +1846,25 @@
         <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H7" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1875,25 +1875,25 @@
         <v>19</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1904,25 +1904,25 @@
         <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1933,25 +1933,25 @@
         <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" t="s">
         <v>118</v>
       </c>
-      <c r="F10" t="s">
-        <v>121</v>
-      </c>
       <c r="G10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1962,25 +1962,25 @@
         <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>26</v>
       </c>
@@ -1991,13 +1991,16 @@
         <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -2008,25 +2011,25 @@
         <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2037,25 +2040,25 @@
         <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2066,25 +2069,25 @@
         <v>33</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2095,25 +2098,25 @@
         <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2124,25 +2127,25 @@
         <v>37</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E17" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H17" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -2153,25 +2156,25 @@
         <v>39</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -2182,25 +2185,25 @@
         <v>41</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2214,33 +2217,33 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="H21" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2251,25 +2254,25 @@
         <v>46</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G22" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H22" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>47</v>
       </c>
@@ -2280,25 +2283,25 @@
         <v>48</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>49</v>
       </c>
@@ -2309,25 +2312,25 @@
         <v>50</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -2338,25 +2341,25 @@
         <v>52</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F25" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G25" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H25" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>53</v>
       </c>
@@ -2367,25 +2370,25 @@
         <v>54</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="F26" s="5" t="s">
+      <c r="I26" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2396,25 +2399,25 @@
         <v>56</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E27" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F27" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G27" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H27" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
@@ -2425,25 +2428,25 @@
         <v>58</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -2454,25 +2457,25 @@
         <v>60</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E29" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F29" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G29" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H29" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -2483,120 +2486,132 @@
         <v>62</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E30" t="s">
         <v>7</v>
       </c>
       <c r="F30" t="s">
+        <v>207</v>
+      </c>
+      <c r="G30" t="s">
+        <v>159</v>
+      </c>
+      <c r="H30" t="s">
+        <v>206</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E31" t="s">
+        <v>212</v>
+      </c>
+      <c r="F31" t="s">
+        <v>211</v>
+      </c>
+      <c r="G31" t="s">
         <v>210</v>
       </c>
-      <c r="G30" t="s">
-        <v>162</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>209</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="8">
-        <v>1</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
         <v>66</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E32" t="s">
+        <v>212</v>
+      </c>
+      <c r="F32" t="s">
         <v>215</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
+        <v>210</v>
+      </c>
+      <c r="H32" t="s">
         <v>214</v>
       </c>
-      <c r="G32" t="s">
+      <c r="I32" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="H32" t="s">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>245</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" t="s">
         <v>212</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="F33" t="s">
+        <v>215</v>
+      </c>
+      <c r="G33" t="s">
+        <v>210</v>
+      </c>
+      <c r="H33" t="s">
+        <v>214</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E33" t="s">
-        <v>215</v>
-      </c>
-      <c r="F33" t="s">
-        <v>218</v>
-      </c>
-      <c r="G33" t="s">
-        <v>213</v>
-      </c>
-      <c r="H33" t="s">
-        <v>217</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
         <v>69</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>70</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E34" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F34" t="s">
         <v>218</v>
       </c>
       <c r="G34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H34" t="s">
         <v>217</v>
@@ -2605,27 +2620,24 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
         <v>71</v>
       </c>
-      <c r="B35">
-        <v>6</v>
-      </c>
-      <c r="C35" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="E35" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="F35" t="s">
+        <v>222</v>
+      </c>
+      <c r="G35" t="s">
         <v>221</v>
-      </c>
-      <c r="G35" t="s">
-        <v>213</v>
       </c>
       <c r="H35" t="s">
         <v>220</v>
@@ -2634,205 +2646,184 @@
         <v>219</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C36" t="s">
         <v>74</v>
       </c>
-      <c r="E36" t="s">
-        <v>227</v>
-      </c>
-      <c r="F36" t="s">
-        <v>225</v>
-      </c>
-      <c r="G36" t="s">
-        <v>224</v>
-      </c>
-      <c r="H36" t="s">
-        <v>223</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" t="s">
+        <v>229</v>
+      </c>
+      <c r="F37" t="s">
+        <v>228</v>
+      </c>
+      <c r="G37" t="s">
+        <v>171</v>
+      </c>
+      <c r="H37" t="s">
+        <v>227</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>78</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>79</v>
-      </c>
-      <c r="E38" t="s">
-        <v>232</v>
-      </c>
-      <c r="F38" t="s">
-        <v>231</v>
-      </c>
-      <c r="G38" t="s">
-        <v>174</v>
-      </c>
-      <c r="H38" t="s">
-        <v>230</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>80</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" t="s">
+        <v>234</v>
+      </c>
+      <c r="F39" t="s">
+        <v>232</v>
+      </c>
+      <c r="G39" t="s">
+        <v>233</v>
+      </c>
+      <c r="H39" t="s">
+        <v>231</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>81</v>
-      </c>
-      <c r="E39" t="s">
-        <v>107</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G39" t="s">
-        <v>105</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>82</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" t="s">
+        <v>234</v>
+      </c>
+      <c r="F40" t="s">
+        <v>232</v>
+      </c>
+      <c r="G40" t="s">
+        <v>233</v>
+      </c>
+      <c r="H40" t="s">
+        <v>231</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>83</v>
-      </c>
-      <c r="E40" t="s">
-        <v>237</v>
-      </c>
-      <c r="F40" t="s">
-        <v>235</v>
-      </c>
-      <c r="G40" t="s">
-        <v>236</v>
-      </c>
-      <c r="H40" t="s">
-        <v>234</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>84</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" t="s">
+        <v>239</v>
+      </c>
+      <c r="F41" t="s">
+        <v>238</v>
+      </c>
+      <c r="G41" t="s">
+        <v>237</v>
+      </c>
+      <c r="H41" t="s">
+        <v>236</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>85</v>
-      </c>
-      <c r="E41" t="s">
-        <v>237</v>
-      </c>
-      <c r="F41" t="s">
-        <v>235</v>
-      </c>
-      <c r="G41" t="s">
-        <v>236</v>
-      </c>
-      <c r="H41" t="s">
-        <v>234</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>86</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E42" t="s">
+        <v>244</v>
+      </c>
+      <c r="F42" t="s">
+        <v>243</v>
+      </c>
+      <c r="G42" t="s">
         <v>242</v>
       </c>
-      <c r="F42" t="s">
+      <c r="H42" t="s">
         <v>241</v>
       </c>
-      <c r="G42" t="s">
+      <c r="I42" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H42" t="s">
-        <v>239</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" t="s">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>223</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
         <v>247</v>
-      </c>
-      <c r="F43" t="s">
-        <v>246</v>
-      </c>
-      <c r="G43" t="s">
-        <v>245</v>
-      </c>
-      <c r="H43" t="s">
-        <v>244</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>226</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2840,7 +2831,7 @@
     <hyperlink ref="E19" r:id="rId1" display="C:\Users\sterl\Downloads\LP L296_EN.pdf" xr:uid="{ADE93B34-E5B6-4AB1-9032-D707F3F99D95}"/>
     <hyperlink ref="I19" r:id="rId2" display="https://www.digikey.com/en/products/detail/osram-opto-semiconductors-inc/LP-L296-J2L2-25-0-20-R18-Z/2205580?s=N4IgTCBcDaIDIAUAEcwE4BsBaAUmVWYArCALoC%2BQA" xr:uid="{95BAC4C6-9E79-4664-B71A-9D2DDD29D800}"/>
     <hyperlink ref="I18" r:id="rId3" display="https://www.digikey.com/en/products/detail/osram-opto-semiconductors-inc/LB-Q39E-N1OO-35-1/2176321" xr:uid="{FF8B05CC-81BB-4F74-AA14-966D5EAB1AA2}"/>
-    <hyperlink ref="I39" r:id="rId4" display="https://www.digikey.com/en/products/detail/amphenol-rf/132134/1011907" xr:uid="{E0955068-F402-4030-A5B7-55613634F68D}"/>
+    <hyperlink ref="I38" r:id="rId4" display="https://www.digikey.com/en/products/detail/amphenol-rf/132134/1011907" xr:uid="{E0955068-F402-4030-A5B7-55613634F68D}"/>
     <hyperlink ref="I3" r:id="rId5" display="https://www.digikey.com/en/products/detail/cal-chip-electronics-inc/GMC10X5R105K16NT/13909090" xr:uid="{5FFF7088-4A7E-4D2A-BC9D-AAAC38BC9037}"/>
     <hyperlink ref="I4" r:id="rId6" display="https://www.digikey.com/en/products/detail/cal-chip-electronics-inc/GMC10X5R226M6R3NT/13909373?s=N4IgTCBcDa4KwHYCMBaA4gWQMJIAwA04AlMMANgzKIGYA5AFXqJVoBEQBdAXyA" xr:uid="{B2DF1EC6-3D93-42DF-BE46-BB1B0238A4FB}"/>
     <hyperlink ref="I9" r:id="rId7" display="https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10C010BB8NNNC/3886753" xr:uid="{7F3CBDC7-177B-4952-9AC8-D869D5C778D4}"/>
@@ -2865,17 +2856,17 @@
     <hyperlink ref="I28" r:id="rId26" display="https://www.digikey.com/en/products/detail/murata-electronics/LQG15HS2N0S02D/1795312?s=N4IgTCBcDaIDIEUDiBGArACQMpgHIAYt8wAREAXQF8g" xr:uid="{83ADC30F-3003-4BF8-9516-37C1CC316AF6}"/>
     <hyperlink ref="I29" r:id="rId27" display="https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/7447860122/12726579" xr:uid="{1A4C2E7A-A72A-42CB-AC2D-4204A7E5E8E8}"/>
     <hyperlink ref="I30" r:id="rId28" display="https://www.digikey.com/en/products/detail/w%C3%BCrth-elektronik/7447860110/12726561" xr:uid="{C70FB2F3-BEF3-4F74-869F-A5757B72438A}"/>
-    <hyperlink ref="I32" r:id="rId29" display="https://www.digikey.com/en/products/detail/nte-electronics-inc/SR1-0603-247/11649452" xr:uid="{A21E807C-2AA0-42A5-9B19-5F33F61CC812}"/>
-    <hyperlink ref="I33" r:id="rId30" display="https://www.digikey.com/en/products/detail/nte-electronics-inc/SR1-0603-610/11655708" xr:uid="{4B4B3456-75B3-4FF6-BAA1-9EC6ECA23EEB}"/>
-    <hyperlink ref="I34" r:id="rId31" display="https://www.digikey.com/en/products/detail/nte-electronics-inc/SR1-0603-610/11655708" xr:uid="{C36112F3-D7BA-42D4-8445-C1C692135910}"/>
-    <hyperlink ref="I35" r:id="rId32" display="https://www.digikey.com/en/products/detail/nte-electronics-inc/SR1-0603-210/11648254" xr:uid="{DE4D8573-8674-41B7-BF8C-8DE6EF07E413}"/>
-    <hyperlink ref="E45" r:id="rId33" xr:uid="{8CFAF093-0074-42A4-9438-6D5F4932F2F5}"/>
-    <hyperlink ref="I36" r:id="rId34" display="https://www.digikey.com/en/products/detail/apem-inc/MJTP1230/1798037" xr:uid="{D7C14627-335E-4BAD-ACCA-1B75D5186982}"/>
-    <hyperlink ref="I38" r:id="rId35" display="https://www.digikey.com/en/products/detail/tdk-corporation/DPX252690DT-5032B1/5819342" xr:uid="{79A7C096-3FC4-42AC-810C-221922A1AF90}"/>
-    <hyperlink ref="I40" r:id="rId36" display="https://www.digikey.com/en/products/detail/adafruit-industries-llc/706/5629413" xr:uid="{DC5EEB89-C1B7-43A9-9151-3C12EFC76064}"/>
-    <hyperlink ref="I41" r:id="rId37" display="https://www.digikey.com/en/products/detail/adafruit-industries-llc/706/5629413" xr:uid="{B99807B2-ACDF-4F6E-A2AA-368AA064244C}"/>
-    <hyperlink ref="I42" r:id="rId38" display="https://www.digikey.com/en/products/detail/epson/FC-135-32-768KA-AG0/3829773" xr:uid="{80E1A1D1-B89C-4EB6-9152-2774F8FBD901}"/>
-    <hyperlink ref="I43" r:id="rId39" display="https://www.digikey.com/en/products/detail/suntsu-electronics-inc/SXT32418FD16-48-000MT/12249197" xr:uid="{7656779F-8039-4B72-B39A-08366BACBE40}"/>
+    <hyperlink ref="I31" r:id="rId29" display="https://www.digikey.com/en/products/detail/nte-electronics-inc/SR1-0603-247/11649452" xr:uid="{A21E807C-2AA0-42A5-9B19-5F33F61CC812}"/>
+    <hyperlink ref="I32" r:id="rId30" display="https://www.digikey.com/en/products/detail/nte-electronics-inc/SR1-0603-610/11655708" xr:uid="{4B4B3456-75B3-4FF6-BAA1-9EC6ECA23EEB}"/>
+    <hyperlink ref="I33" r:id="rId31" display="https://www.digikey.com/en/products/detail/nte-electronics-inc/SR1-0603-610/11655708" xr:uid="{C36112F3-D7BA-42D4-8445-C1C692135910}"/>
+    <hyperlink ref="I34" r:id="rId32" display="https://www.digikey.com/en/products/detail/nte-electronics-inc/SR1-0603-210/11648254" xr:uid="{DE4D8573-8674-41B7-BF8C-8DE6EF07E413}"/>
+    <hyperlink ref="E44" r:id="rId33" xr:uid="{8CFAF093-0074-42A4-9438-6D5F4932F2F5}"/>
+    <hyperlink ref="I35" r:id="rId34" display="https://www.digikey.com/en/products/detail/apem-inc/MJTP1230/1798037" xr:uid="{D7C14627-335E-4BAD-ACCA-1B75D5186982}"/>
+    <hyperlink ref="I37" r:id="rId35" display="https://www.digikey.com/en/products/detail/tdk-corporation/DPX252690DT-5032B1/5819342" xr:uid="{79A7C096-3FC4-42AC-810C-221922A1AF90}"/>
+    <hyperlink ref="I39" r:id="rId36" display="https://www.digikey.com/en/products/detail/adafruit-industries-llc/706/5629413" xr:uid="{DC5EEB89-C1B7-43A9-9151-3C12EFC76064}"/>
+    <hyperlink ref="I40" r:id="rId37" display="https://www.digikey.com/en/products/detail/adafruit-industries-llc/706/5629413" xr:uid="{B99807B2-ACDF-4F6E-A2AA-368AA064244C}"/>
+    <hyperlink ref="I41" r:id="rId38" display="https://www.digikey.com/en/products/detail/epson/FC-135-32-768KA-AG0/3829773" xr:uid="{80E1A1D1-B89C-4EB6-9152-2774F8FBD901}"/>
+    <hyperlink ref="I42" r:id="rId39" display="https://www.digikey.com/en/products/detail/suntsu-electronics-inc/SXT32418FD16-48-000MT/12249197" xr:uid="{7656779F-8039-4B72-B39A-08366BACBE40}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId40"/>

</xml_diff>